<commit_message>
1. add a weights function, but need to think about how to evaluate weight of samples., and how to combine. Till now, if simply based on RE, not effective, if too sparse, worse. 2. try to pre training to calibrate sensor response, but need to think how to apply calibration on test_param 3. try boosting and bagging, not better 4. Add tansig in DNN and not that effective for C6H6
</commit_message>
<xml_diff>
--- a/EXP.xlsx
+++ b/EXP.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
   <si>
     <t>RF1,3,5,T,RH,AH -&gt; S1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -214,6 +214,18 @@
   </si>
   <si>
     <t>lassoCV(cv = 1, normalize)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tansig*2,  输出不经过norm, hw=5, 8000(已收敛)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bagging</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -551,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1215,7 +1227,7 @@
         <v>-1.9599999999999999E-2</v>
       </c>
       <c r="L16" s="2">
-        <v>0.42030000000000001</v>
+        <v>0.42303000000000002</v>
       </c>
       <c r="N16" t="s">
         <v>22</v>
@@ -1248,7 +1260,7 @@
         <v>5.1799999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="8:24" x14ac:dyDescent="0.2">
       <c r="I17" t="s">
         <v>16</v>
       </c>
@@ -1259,7 +1271,7 @@
         <v>-1.9599999999999999E-2</v>
       </c>
       <c r="L17" s="2">
-        <v>0.42030000000000001</v>
+        <v>0.42303000000000002</v>
       </c>
       <c r="N17" t="s">
         <v>23</v>
@@ -1278,7 +1290,7 @@
       </c>
       <c r="U17"/>
     </row>
-    <row r="18" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="8:24" x14ac:dyDescent="0.2">
       <c r="H18" t="s">
         <v>45</v>
       </c>
@@ -1310,7 +1322,7 @@
         <v>3.4299999999999997E-2</v>
       </c>
     </row>
-    <row r="19" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="8:24" x14ac:dyDescent="0.2">
       <c r="I19" t="s">
         <v>18</v>
       </c>
@@ -1324,7 +1336,7 @@
         <v>0.43690000000000001</v>
       </c>
     </row>
-    <row r="20" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="8:24" x14ac:dyDescent="0.2">
       <c r="I20" t="s">
         <v>15</v>
       </c>
@@ -1338,7 +1350,7 @@
         <v>0.43690000000000001</v>
       </c>
     </row>
-    <row r="21" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="8:24" x14ac:dyDescent="0.2">
       <c r="I21" t="s">
         <v>48</v>
       </c>
@@ -1352,7 +1364,7 @@
         <v>0.43980000000000002</v>
       </c>
     </row>
-    <row r="22" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="8:24" x14ac:dyDescent="0.2">
       <c r="I22" t="s">
         <v>16</v>
       </c>
@@ -1366,12 +1378,49 @@
         <v>0.43980000000000002</v>
       </c>
     </row>
-    <row r="25" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="8:24" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="K23" s="2">
+        <v>-8.9999999999999998E-4</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0.42059999999999997</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0.2298</v>
+      </c>
+      <c r="T23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="8:24" x14ac:dyDescent="0.2">
+      <c r="T24" t="s">
+        <v>50</v>
+      </c>
+      <c r="U24" s="2">
+        <v>0.31707965625599999</v>
+      </c>
+      <c r="V24" s="2">
+        <v>1.42910258876</v>
+      </c>
+      <c r="W24" s="2">
+        <v>0.115775787968</v>
+      </c>
+      <c r="X24" s="2">
+        <v>0.13396664999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="8:24" x14ac:dyDescent="0.2">
       <c r="M25" s="2">
         <v>0.244754281289642</v>
       </c>
     </row>
-    <row r="27" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="8:24" x14ac:dyDescent="0.2">
       <c r="J27" s="2">
         <v>0.30399999999999999</v>
       </c>
@@ -1382,7 +1431,7 @@
         <v>0.43919999999999998</v>
       </c>
     </row>
-    <row r="28" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="8:24" x14ac:dyDescent="0.2">
       <c r="I28" t="s">
         <v>44</v>
       </c>
@@ -1399,7 +1448,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="8:24" x14ac:dyDescent="0.2">
       <c r="I29" t="s">
         <v>28</v>
       </c>
@@ -1416,7 +1465,7 @@
         <v>0.19600000000000001</v>
       </c>
     </row>
-    <row r="30" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="8:24" x14ac:dyDescent="0.2">
       <c r="I30" t="s">
         <v>29</v>
       </c>
@@ -1433,7 +1482,7 @@
         <v>0.2737</v>
       </c>
     </row>
-    <row r="31" spans="8:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="8:24" x14ac:dyDescent="0.2">
       <c r="I31" t="s">
         <v>43</v>
       </c>

</xml_diff>